<commit_message>
index and sput upd
Восстановили полную работоспособность индексов, а так же улучшили бд
</commit_message>
<xml_diff>
--- a/sput.xlsx
+++ b/sput.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="183">
   <si>
     <t>Intelsat 22</t>
   </si>
@@ -30,9 +30,6 @@
     <t>Ku</t>
   </si>
   <si>
-    <t>Intelsat 20</t>
-  </si>
-  <si>
     <t>CKu</t>
   </si>
   <si>
@@ -87,39 +84,18 @@
     <t>Express AM7</t>
   </si>
   <si>
-    <t>Hellas Sat 3</t>
-  </si>
-  <si>
     <t>Paksat MM1</t>
   </si>
   <si>
     <t>Paksat 1R</t>
   </si>
   <si>
-    <t>Express AMU1 (Eutelsat 36C)</t>
-  </si>
-  <si>
     <t>Eutelsat 36B</t>
   </si>
   <si>
-    <t>Eutelsat 33F</t>
-  </si>
-  <si>
-    <t>Arabsat 5A</t>
-  </si>
-  <si>
-    <t>Astra 2E (Eutelsat 28E)</t>
-  </si>
-  <si>
-    <t>Badr 5</t>
-  </si>
-  <si>
     <t>Es'hail 1</t>
   </si>
   <si>
-    <t>Astra 3B</t>
-  </si>
-  <si>
     <t>Angosat 2</t>
   </si>
   <si>
@@ -129,57 +105,21 @@
     <t>Arabsat 5C</t>
   </si>
   <si>
-    <t>Astra 1KR</t>
-  </si>
-  <si>
     <t>Amos 17</t>
   </si>
   <si>
     <t>Eutelsat 16A</t>
   </si>
   <si>
-    <t>Hotbird 13F</t>
-  </si>
-  <si>
     <t>Eutelsat 10B</t>
   </si>
   <si>
-    <t>Eutelsat Ka-Sat 9A</t>
-  </si>
-  <si>
     <t>Ka</t>
   </si>
   <si>
-    <t>Eutelsat 7B</t>
-  </si>
-  <si>
-    <t>SES 5</t>
-  </si>
-  <si>
-    <t>Eutelsat 3B</t>
-  </si>
-  <si>
     <t>BulgariaSat 1</t>
   </si>
   <si>
-    <t>G-Sat 8 (incl. 0.4°)</t>
-  </si>
-  <si>
-    <t>TurkmenДlem/MonacoSat</t>
-  </si>
-  <si>
-    <t>Tьrksat 4B</t>
-  </si>
-  <si>
-    <t>Tьrksat 6A</t>
-  </si>
-  <si>
-    <t>Tьrksat 5B</t>
-  </si>
-  <si>
-    <t>Tьrksat 5A</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
@@ -331,13 +271,964 @@
   </si>
   <si>
     <t>latitude</t>
+  </si>
+  <si>
+    <t>Names</t>
+  </si>
+  <si>
+    <t>Intelsat 20/36</t>
+  </si>
+  <si>
+    <t>G-Sat 8/16, Yamal 402</t>
+  </si>
+  <si>
+    <t>Türksat 3A/4A/5B</t>
+  </si>
+  <si>
+    <t>Türksat  4B</t>
+  </si>
+  <si>
+    <t>Türksat  6A</t>
+  </si>
+  <si>
+    <t>Hellas Sat 3/4</t>
+  </si>
+  <si>
+    <t>Express AMU1 (Eutelsat 36C/36D)</t>
+  </si>
+  <si>
+    <t>Türksat 5A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eutelsat 33F, Intelsat 28 </t>
+  </si>
+  <si>
+    <t>Arabsat 5A/6A</t>
+  </si>
+  <si>
+    <t>Astra 2E/F/G (Eutelsat 28E/F/G)</t>
+  </si>
+  <si>
+    <t>Badr 5/7/8, Es'hail 2</t>
+  </si>
+  <si>
+    <t>Astra 3B/C</t>
+  </si>
+  <si>
+    <t>Astra 1KR/L/M/N</t>
+  </si>
+  <si>
+    <t>Hotbird 13F/G</t>
+  </si>
+  <si>
+    <t>Eutelsat 7B/C</t>
+  </si>
+  <si>
+    <t>Eutelsat Ka-Sat 9A, Eutelsat 9B</t>
+  </si>
+  <si>
+    <t>SES 5, Astra 4A</t>
+  </si>
+  <si>
+    <t>Eutelsat 3B, Rascom QAF 1R</t>
+  </si>
+  <si>
+    <t>TurkmenÄlem/MonacoSat</t>
+  </si>
+  <si>
+    <t>NSS 9</t>
+  </si>
+  <si>
+    <t>Intelsat 18</t>
+  </si>
+  <si>
+    <t>Eutelsat 172B</t>
+  </si>
+  <si>
+    <t>Horizons 3e</t>
+  </si>
+  <si>
+    <t>Intelsat 19</t>
+  </si>
+  <si>
+    <t>ChinaSat 19</t>
+  </si>
+  <si>
+    <t>Superbird B3</t>
+  </si>
+  <si>
+    <r>
+      <t>Optus D2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <u/>
+        <sz val="7.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>(incl. 0.5°)</t>
+    </r>
+  </si>
+  <si>
+    <t>Measat 3a</t>
+  </si>
+  <si>
+    <t>ABS 6</t>
+  </si>
+  <si>
+    <r>
+      <t>Optus D3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <u/>
+        <sz val="7.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>(incl. 0.3°)</t>
+    </r>
+  </si>
+  <si>
+    <t>Optus 10</t>
+  </si>
+  <si>
+    <t>JCSAT 2B</t>
+  </si>
+  <si>
+    <r>
+      <t>Optus D1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <u/>
+        <sz val="7.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>(incl. 1.5°)</t>
+    </r>
+  </si>
+  <si>
+    <t>BRIsat</t>
+  </si>
+  <si>
+    <t>JCSAT 1C</t>
+  </si>
+  <si>
+    <t>Nusantara Satu</t>
+  </si>
+  <si>
+    <t>Express AMU7</t>
+  </si>
+  <si>
+    <t>JCSAT 16</t>
+  </si>
+  <si>
+    <r>
+      <t>Superbird C2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <u/>
+        <sz val="7.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>(incl. 0.8°)</t>
+    </r>
+  </si>
+  <si>
+    <t>Apstar 9</t>
+  </si>
+  <si>
+    <t>Express AM5</t>
+  </si>
+  <si>
+    <t>Express AT2</t>
+  </si>
+  <si>
+    <t>Telstar 18 Vantage (Apstar 5C)</t>
+  </si>
+  <si>
+    <r>
+      <t>134.</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="7.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>°E</t>
+    </r>
+  </si>
+  <si>
+    <t>Apstar 6E</t>
+  </si>
+  <si>
+    <t>Apstar 6D</t>
+  </si>
+  <si>
+    <t>Apstar 6C</t>
+  </si>
+  <si>
+    <r>
+      <t>132.</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="7.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>°E</t>
+    </r>
+  </si>
+  <si>
+    <t>JCSAT 12</t>
+  </si>
+  <si>
+    <t>JCSAT 5A</t>
+  </si>
+  <si>
+    <t>Vinasat 1</t>
+  </si>
+  <si>
+    <t>Vinasat 2</t>
+  </si>
+  <si>
+    <r>
+      <t>130.</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="7.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>5</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>°E</t>
+    </r>
+  </si>
+  <si>
+    <t>ChinaSat 6C</t>
+  </si>
+  <si>
+    <r>
+      <t>130.</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="7.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>°E</t>
+    </r>
+  </si>
+  <si>
+    <t>ChinaSat 2D</t>
+  </si>
+  <si>
+    <r>
+      <t>128.</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="7.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>5</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>°E</t>
+    </r>
+  </si>
+  <si>
+    <t>LaoSat 1</t>
+  </si>
+  <si>
+    <r>
+      <t>128.</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="7.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>°E</t>
+    </r>
+  </si>
+  <si>
+    <t>JCSAT 3A</t>
+  </si>
+  <si>
+    <t>Cosmos 2526</t>
+  </si>
+  <si>
+    <r>
+      <t>125.</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="7.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>°E</t>
+    </r>
+  </si>
+  <si>
+    <t>ChinaSat 6D</t>
+  </si>
+  <si>
+    <r>
+      <t>124.</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="7.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>°E</t>
+    </r>
+  </si>
+  <si>
+    <t>JCSAT 4B</t>
+  </si>
+  <si>
+    <r>
+      <t>122.</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="7.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>°E</t>
+    </r>
+  </si>
+  <si>
+    <t>AsiaSat 9</t>
+  </si>
+  <si>
+    <r>
+      <t>120.</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="7.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>°E</t>
+    </r>
+  </si>
+  <si>
+    <t>AsiaSat 6/Thaicom 7</t>
+  </si>
+  <si>
+    <r>
+      <t>119.</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="7.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>°E</t>
+    </r>
+  </si>
+  <si>
+    <t>Thaicom 4</t>
+  </si>
+  <si>
+    <t>Bangabandhu 1</t>
+  </si>
+  <si>
+    <r>
+      <t>118.</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="7.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>°E</t>
+    </r>
+  </si>
+  <si>
+    <t>ChinaSat 4A</t>
+  </si>
+  <si>
+    <t>Telkom 3S</t>
+  </si>
+  <si>
+    <r>
+      <t>177.</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="7.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>180.</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="7.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>172.</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="7.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>169.</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="7.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>166.</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="7.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>163.</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="7.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>162.</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="7.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>160.</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="7.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>159.</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="7.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>156.</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="7.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>154.</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="7.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>152.</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="7.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>150.</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="7.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>5</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>150.</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="7.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>146.</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="7.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>145.</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="7.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>144.</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="7.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>140.</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="7.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>142.</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="7.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>138.</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="7.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>134.</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="7.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>0</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -353,6 +1244,52 @@
       <family val="2"/>
       <charset val="204"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="7.5"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="7.5"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="7.5"/>
+      <color theme="1"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <i/>
+      <u/>
+      <sz val="7.5"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="2">
@@ -375,13 +1312,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -676,34 +1620,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F51"/>
+  <dimension ref="A1:M95"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J40" sqref="J40"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="D75" sqref="D75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="17.28515625" customWidth="1"/>
-    <col min="2" max="2" width="60.42578125" customWidth="1"/>
+    <col min="2" max="2" width="30.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29" customWidth="1"/>
+    <col min="6" max="6" width="10" customWidth="1"/>
+    <col min="9" max="9" width="35" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="B1" t="s">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>104</v>
+        <v>84</v>
       </c>
       <c r="D1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+        <v>36</v>
+      </c>
+      <c r="I1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -714,7 +1663,7 @@
         <v>0</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="E2" t="s">
         <v>1</v>
@@ -722,8 +1671,12 @@
       <c r="F2">
         <v>241006</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="I2" t="str">
+        <f>CONCATENATE(D2, " ",B2)</f>
+        <v>72.1 Intelsat 22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -734,7 +1687,7 @@
         <v>0</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="E3" t="s">
         <v>3</v>
@@ -742,59 +1695,72 @@
       <c r="F3">
         <v>240821</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="I3" t="str">
+        <f t="shared" ref="I3:I50" si="0">CONCATENATE(D3, " ",B3)</f>
+        <v>70.5 Eutelsat 70B</v>
+      </c>
+      <c r="M3" s="2"/>
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" t="s">
         <v>4</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="E4" t="s">
-        <v>5</v>
       </c>
       <c r="F4">
         <v>241007</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="I4" t="str">
+        <f t="shared" si="0"/>
+        <v>68.5 Intelsat 20/36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5">
         <v>0</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="E5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F5">
         <v>240929</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="I5" t="str">
+        <f t="shared" si="0"/>
+        <v>66.0 Intelsat 17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6">
         <v>0</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>61</v>
+        <v>41</v>
       </c>
       <c r="E6" t="s">
         <v>3</v>
@@ -802,59 +1768,71 @@
       <c r="F6">
         <v>240909</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="I6" t="str">
+        <f t="shared" si="0"/>
+        <v>65.0 Amos 4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C7">
         <v>0</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>62</v>
+        <v>42</v>
       </c>
       <c r="E7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F7">
         <v>241005</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="I7" t="str">
+        <f t="shared" si="0"/>
+        <v>62.0 Intelsat 39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>63</v>
+        <v>43</v>
       </c>
       <c r="E8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F8">
         <v>240623</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="I8" t="str">
+        <f t="shared" si="0"/>
+        <v>60.0 Intelsat 33e</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C9">
         <v>0</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="E9" t="s">
         <v>3</v>
@@ -862,39 +1840,47 @@
       <c r="F9">
         <v>241001</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="I9" t="str">
+        <f t="shared" si="0"/>
+        <v>58.5 KazSat 3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C10">
         <v>0</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="E10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F10">
         <v>241010</v>
       </c>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="I10" t="str">
+        <f t="shared" si="0"/>
+        <v>57.0 NSS 12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
       <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C11">
         <v>0</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>66</v>
+        <v>46</v>
       </c>
       <c r="E11" t="s">
         <v>3</v>
@@ -902,19 +1888,23 @@
       <c r="F11">
         <v>241009</v>
       </c>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="I11" t="str">
+        <f t="shared" si="0"/>
+        <v>56.0 Express AT1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
       <c r="A12" s="1">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>48</v>
+        <v>87</v>
       </c>
       <c r="C12">
         <v>0</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="E12" t="s">
         <v>3</v>
@@ -922,19 +1912,23 @@
       <c r="F12">
         <v>241010</v>
       </c>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="I12" t="str">
+        <f t="shared" si="0"/>
+        <v>55.0 G-Sat 8/16, Yamal 402</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
       <c r="A13" s="1">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C13">
         <v>0</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>68</v>
+        <v>48</v>
       </c>
       <c r="E13" t="s">
         <v>3</v>
@@ -942,19 +1936,23 @@
       <c r="F13">
         <v>241010</v>
       </c>
-    </row>
-    <row r="14" spans="1:6">
+      <c r="I13" t="str">
+        <f t="shared" si="0"/>
+        <v>53.0 Express AM6 (Eutelsat 53A)</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
       <c r="A14" s="1">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C14">
         <v>0</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>69</v>
+        <v>49</v>
       </c>
       <c r="E14" t="s">
         <v>3</v>
@@ -962,19 +1960,23 @@
       <c r="F14">
         <v>241006</v>
       </c>
-    </row>
-    <row r="15" spans="1:6">
+      <c r="I14" t="str">
+        <f t="shared" si="0"/>
+        <v>52.5 Al Yah 1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
       <c r="A15" s="1">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>49</v>
+        <v>105</v>
       </c>
       <c r="C15">
         <v>0</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="E15" t="s">
         <v>3</v>
@@ -982,39 +1984,47 @@
       <c r="F15">
         <v>241006</v>
       </c>
-    </row>
-    <row r="16" spans="1:6">
+      <c r="I15" t="str">
+        <f t="shared" si="0"/>
+        <v>52.0 TurkmenÄlem/MonacoSat</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
       <c r="A16" s="1">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C16">
         <v>0</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="E16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F16">
         <v>240917</v>
       </c>
-    </row>
-    <row r="17" spans="1:6">
+      <c r="I16" t="str">
+        <f t="shared" si="0"/>
+        <v>51.5 Belintersat 1 (ChinaSat 15)</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17" s="1">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>50</v>
+        <v>89</v>
       </c>
       <c r="C17">
         <v>0</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="E17" t="s">
         <v>3</v>
@@ -1022,33 +2032,41 @@
       <c r="F17">
         <v>230819</v>
       </c>
-    </row>
-    <row r="18" spans="1:6">
+      <c r="I17" t="str">
+        <f t="shared" si="0"/>
+        <v>50.0 Türksat  4B</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18" s="1">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>51</v>
+        <v>90</v>
       </c>
       <c r="C18">
         <v>0</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
+        <v>52</v>
+      </c>
+      <c r="I18" t="str">
+        <f t="shared" si="0"/>
+        <v>50.0 Türksat  6A</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19" s="1">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C19">
         <v>0</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>73</v>
+        <v>53</v>
       </c>
       <c r="E19" t="s">
         <v>1</v>
@@ -1056,39 +2074,47 @@
       <c r="F19">
         <v>241010</v>
       </c>
-    </row>
-    <row r="20" spans="1:6">
+      <c r="I19" t="str">
+        <f t="shared" si="0"/>
+        <v>49.0 Yamal 601</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
       <c r="A20" s="1">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C20">
         <v>0</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>74</v>
+        <v>54</v>
       </c>
       <c r="E20" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F20">
         <v>241010</v>
       </c>
-    </row>
-    <row r="21" spans="1:6">
+      <c r="I20" t="str">
+        <f t="shared" si="0"/>
+        <v>46.0 Azerspace 1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
       <c r="A21" s="1">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C21">
         <v>0</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="E21" t="s">
         <v>3</v>
@@ -1096,53 +2122,65 @@
       <c r="F21">
         <v>241005</v>
       </c>
-    </row>
-    <row r="22" spans="1:6">
+      <c r="I21" t="str">
+        <f t="shared" si="0"/>
+        <v>45.1 Azerspace 2/Intelsat 38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
       <c r="A22" s="1">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C22">
         <v>0</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
+        <v>56</v>
+      </c>
+      <c r="I22" t="str">
+        <f t="shared" si="0"/>
+        <v>45.0 Cosmos 2520</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
       <c r="A23" s="1">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C23">
         <v>0</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>77</v>
+        <v>57</v>
       </c>
       <c r="E23" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F23">
         <v>240622</v>
       </c>
-    </row>
-    <row r="24" spans="1:6">
+      <c r="I23" t="str">
+        <f t="shared" si="0"/>
+        <v>42.5 NigComSat 1R</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
       <c r="A24" s="1">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>52</v>
+        <v>88</v>
       </c>
       <c r="C24">
         <v>0</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="E24" t="s">
         <v>3</v>
@@ -1150,39 +2188,47 @@
       <c r="F24">
         <v>240929</v>
       </c>
-    </row>
-    <row r="25" spans="1:6">
+      <c r="I24" t="str">
+        <f t="shared" si="0"/>
+        <v>42.0 Türksat 3A/4A/5B</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
       <c r="A25" s="1">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C25">
         <v>0</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>79</v>
+        <v>59</v>
       </c>
       <c r="E25" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F25">
         <v>241010</v>
       </c>
-    </row>
-    <row r="26" spans="1:6">
+      <c r="I25" t="str">
+        <f t="shared" si="0"/>
+        <v>40.0 Express AM7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
       <c r="A26" s="1">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>23</v>
+        <v>91</v>
       </c>
       <c r="C26">
         <v>0</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="E26" t="s">
         <v>3</v>
@@ -1190,53 +2236,65 @@
       <c r="F26">
         <v>241006</v>
       </c>
-    </row>
-    <row r="27" spans="1:6">
+      <c r="I26" t="str">
+        <f t="shared" si="0"/>
+        <v>39.0 Hellas Sat 3/4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
       <c r="A27" s="1">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C27">
         <v>0</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
+        <v>61</v>
+      </c>
+      <c r="I27" t="str">
+        <f t="shared" si="0"/>
+        <v>38.2 Paksat MM1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
       <c r="A28" s="1">
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C28">
         <v>0</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>82</v>
+        <v>62</v>
       </c>
       <c r="E28" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F28">
         <v>240923</v>
       </c>
-    </row>
-    <row r="29" spans="1:6">
+      <c r="I28" t="str">
+        <f t="shared" si="0"/>
+        <v>38.0 Paksat 1R</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
       <c r="A29" s="1">
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>26</v>
+        <v>92</v>
       </c>
       <c r="C29">
         <v>0</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>83</v>
+        <v>63</v>
       </c>
       <c r="E29" t="s">
         <v>3</v>
@@ -1244,33 +2302,41 @@
       <c r="F29">
         <v>241010</v>
       </c>
-    </row>
-    <row r="30" spans="1:6">
+      <c r="I29" t="str">
+        <f t="shared" si="0"/>
+        <v>36.0 Express AMU1 (Eutelsat 36C/36D)</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
       <c r="A30" s="1">
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C30">
         <v>0</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
+        <v>63</v>
+      </c>
+      <c r="I30" t="str">
+        <f t="shared" si="0"/>
+        <v>36.0 Eutelsat 36B</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
       <c r="A31" s="1">
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>28</v>
+        <v>94</v>
       </c>
       <c r="C31">
         <v>0</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="E31" t="s">
         <v>3</v>
@@ -1278,36 +2344,44 @@
       <c r="F31">
         <v>240922</v>
       </c>
-    </row>
-    <row r="32" spans="1:6">
+      <c r="I31" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">33.0 Eutelsat 33F, Intelsat 28 </v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
       <c r="A32" s="1">
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>53</v>
+        <v>93</v>
       </c>
       <c r="C32">
         <v>0</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="E32" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="33" spans="1:6">
+      <c r="I32" t="str">
+        <f t="shared" si="0"/>
+        <v>31.0 Türksat 5A</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
       <c r="A33" s="1">
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>29</v>
+        <v>95</v>
       </c>
       <c r="C33">
         <v>0</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>86</v>
+        <v>66</v>
       </c>
       <c r="E33" t="s">
         <v>3</v>
@@ -1315,70 +2389,86 @@
       <c r="F33">
         <v>240928</v>
       </c>
-    </row>
-    <row r="34" spans="1:6">
+      <c r="I33" t="str">
+        <f t="shared" si="0"/>
+        <v>30.5 Arabsat 5A/6A</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
       <c r="A34" s="1">
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>30</v>
+        <v>96</v>
       </c>
       <c r="C34">
         <v>0</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>87</v>
+        <v>67</v>
       </c>
       <c r="E34" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="35" spans="1:6">
+      <c r="I34" t="str">
+        <f t="shared" si="0"/>
+        <v>28.3 Astra 2E/F/G (Eutelsat 28E/F/G)</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
       <c r="A35" s="1">
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>31</v>
+        <v>97</v>
       </c>
       <c r="C35">
         <v>0</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="E35" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="36" spans="1:6">
+      <c r="I35" t="str">
+        <f t="shared" si="0"/>
+        <v>26.0 Badr 5/7/8, Es'hail 2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
       <c r="A36" s="1">
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C36">
         <v>0</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
       <c r="E36" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
+        <v>20</v>
+      </c>
+      <c r="I36" t="str">
+        <f t="shared" si="0"/>
+        <v>25.5 Es'hail 1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
       <c r="A37" s="1">
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>33</v>
+        <v>98</v>
       </c>
       <c r="C37">
         <v>0</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="E37" t="s">
         <v>3</v>
@@ -1386,50 +2476,62 @@
       <c r="F37">
         <v>240717</v>
       </c>
-    </row>
-    <row r="38" spans="1:6">
+      <c r="I37" t="str">
+        <f t="shared" si="0"/>
+        <v>23.5 Astra 3B/C</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
       <c r="A38" s="1">
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C38">
         <v>0</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6">
+        <v>71</v>
+      </c>
+      <c r="I38" t="str">
+        <f t="shared" si="0"/>
+        <v>23.0 Angosat 2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
       <c r="A39" s="1">
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C39">
         <v>0</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>92</v>
+        <v>72</v>
       </c>
       <c r="E39" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="40" spans="1:6">
+      <c r="I39" t="str">
+        <f t="shared" si="0"/>
+        <v>21.5 Eutelsat 21B</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
       <c r="A40" s="1">
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C40">
         <v>0</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
       <c r="E40" t="s">
         <v>1</v>
@@ -1437,19 +2539,23 @@
       <c r="F40">
         <v>241003</v>
       </c>
-    </row>
-    <row r="41" spans="1:6">
+      <c r="I40" t="str">
+        <f t="shared" si="0"/>
+        <v>20.0 Arabsat 5C</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
       <c r="A41" s="1">
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>37</v>
+        <v>99</v>
       </c>
       <c r="C41">
         <v>0</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>94</v>
+        <v>74</v>
       </c>
       <c r="E41" t="s">
         <v>3</v>
@@ -1457,56 +2563,68 @@
       <c r="F41">
         <v>241006</v>
       </c>
-    </row>
-    <row r="42" spans="1:6">
+      <c r="I41" t="str">
+        <f t="shared" si="0"/>
+        <v>19.2 Astra 1KR/L/M/N</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
       <c r="A42" s="1">
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="C42">
         <v>0</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>95</v>
+        <v>75</v>
       </c>
       <c r="E42" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6">
+        <v>4</v>
+      </c>
+      <c r="I42" t="str">
+        <f t="shared" si="0"/>
+        <v>17.0 Amos 17</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9">
       <c r="A43" s="1">
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="C43">
         <v>0</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>96</v>
+        <v>76</v>
       </c>
       <c r="E43" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F43">
         <v>240818</v>
       </c>
-    </row>
-    <row r="44" spans="1:6">
+      <c r="I43" t="str">
+        <f t="shared" si="0"/>
+        <v>16.0 Eutelsat 16A</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9">
       <c r="A44" s="1">
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="C44">
         <v>0</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>97</v>
+        <v>77</v>
       </c>
       <c r="E44" t="s">
         <v>3</v>
@@ -1514,107 +2632,131 @@
       <c r="F44">
         <v>241010</v>
       </c>
-    </row>
-    <row r="45" spans="1:6">
+      <c r="I44" t="str">
+        <f t="shared" si="0"/>
+        <v>13.0 Hotbird 13F/G</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
       <c r="A45" s="1">
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C45">
         <v>0</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>98</v>
+        <v>78</v>
       </c>
       <c r="E45" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6">
+        <v>4</v>
+      </c>
+      <c r="I45" t="str">
+        <f t="shared" si="0"/>
+        <v>10.0 Eutelsat 10B</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9">
       <c r="A46" s="1">
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>42</v>
+        <v>102</v>
       </c>
       <c r="C46">
         <v>0</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>99</v>
+        <v>79</v>
       </c>
       <c r="E46" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="F46">
         <v>241003</v>
       </c>
-    </row>
-    <row r="47" spans="1:6">
+      <c r="I46" t="str">
+        <f t="shared" si="0"/>
+        <v>9.0 Eutelsat Ka-Sat 9A, Eutelsat 9B</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9">
       <c r="A47" s="1">
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>44</v>
+        <v>101</v>
       </c>
       <c r="C47">
         <v>0</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="E47" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6">
+        <v>20</v>
+      </c>
+      <c r="I47" t="str">
+        <f t="shared" si="0"/>
+        <v>7.0 Eutelsat 7B/C</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9">
       <c r="A48" s="1">
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>45</v>
+        <v>103</v>
       </c>
       <c r="C48">
         <v>0</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="E48" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6">
+        <v>4</v>
+      </c>
+      <c r="I48" t="str">
+        <f t="shared" si="0"/>
+        <v>4.9 SES 5, Astra 4A</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9">
       <c r="A49" s="1">
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>46</v>
+        <v>104</v>
       </c>
       <c r="C49">
         <v>0</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>102</v>
+        <v>82</v>
       </c>
       <c r="E49" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6">
+        <v>4</v>
+      </c>
+      <c r="I49" t="str">
+        <f t="shared" si="0"/>
+        <v>3.0 Eutelsat 3B, Rascom QAF 1R</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9">
       <c r="A50" s="1">
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="C50">
         <v>0</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="E50" t="s">
         <v>3</v>
@@ -1622,13 +2764,872 @@
       <c r="F50">
         <v>240921</v>
       </c>
-    </row>
-    <row r="51" spans="1:6">
-      <c r="A51" s="1"/>
+      <c r="I50" t="str">
+        <f t="shared" si="0"/>
+        <v>1.9 BulgariaSat 1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9">
+      <c r="A51" s="1">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>106</v>
+      </c>
+      <c r="C51" s="4"/>
+      <c r="D51" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E51" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F51" s="6">
+        <v>240702</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9">
+      <c r="A52" s="1">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>107</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="E52" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F52" s="6">
+        <v>240904</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9">
+      <c r="A53" s="1">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>108</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="E53" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F53" s="6">
+        <v>241101</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9">
+      <c r="A54" s="1">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>109</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="E54" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F54" s="6">
+        <v>240915</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9">
+      <c r="A55" s="1">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>110</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="E55" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F55" s="6">
+        <v>241104</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9">
+      <c r="A56" s="1">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>111</v>
+      </c>
+      <c r="C56" s="4"/>
+      <c r="D56" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="E56" s="5"/>
+      <c r="F56" s="6"/>
+    </row>
+    <row r="57" spans="1:9">
+      <c r="A57" s="1">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>112</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="E57" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F57" s="6">
+        <v>201122</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9">
+      <c r="A58" s="1">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>113</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="E58" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F58" s="6">
+        <v>241013</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9">
+      <c r="A59" s="1">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>114</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+      <c r="D59" s="2"/>
+      <c r="E59" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F59" s="6">
+        <v>240808</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9">
+      <c r="A60" s="1">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>115</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="E60" s="5"/>
+      <c r="F60" s="6">
+        <v>240917</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9">
+      <c r="A61" s="1">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>116</v>
+      </c>
+      <c r="C61" s="4"/>
+      <c r="D61" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="E61" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F61" s="6">
+        <v>240926</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9">
+      <c r="A62" s="1">
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>117</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
+      <c r="D62" s="2"/>
+      <c r="E62" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F62" s="6">
+        <v>240916</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9">
+      <c r="A63" s="1">
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
+        <v>118</v>
+      </c>
+      <c r="C63">
+        <v>0</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="E63" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F63" s="6">
+        <v>240515</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9">
+      <c r="A64" s="1">
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>119</v>
+      </c>
+      <c r="C64">
+        <v>0</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="E64" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F64" s="6">
+        <v>241111</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6">
+      <c r="A65" s="1">
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
+        <v>120</v>
+      </c>
+      <c r="C65">
+        <v>0</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="E65" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F65" s="6">
+        <v>240304</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6">
+      <c r="A66" s="1">
+        <v>65</v>
+      </c>
+      <c r="B66" t="s">
+        <v>121</v>
+      </c>
+      <c r="C66" s="4"/>
+      <c r="D66" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="E66" s="5"/>
+      <c r="F66" s="6"/>
+    </row>
+    <row r="67" spans="1:6">
+      <c r="A67" s="1">
+        <v>66</v>
+      </c>
+      <c r="B67" t="s">
+        <v>122</v>
+      </c>
+      <c r="C67">
+        <v>0</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="E67" s="5"/>
+      <c r="F67" s="6">
+        <v>240816</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6">
+      <c r="A68" s="1">
+        <v>67</v>
+      </c>
+      <c r="B68" t="s">
+        <v>123</v>
+      </c>
+      <c r="C68">
+        <v>0</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="E68" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F68" s="6">
+        <v>241006</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6">
+      <c r="A69" s="1">
+        <v>68</v>
+      </c>
+      <c r="B69" t="s">
+        <v>124</v>
+      </c>
+      <c r="C69">
+        <v>0</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="E69" s="5"/>
+      <c r="F69" s="6"/>
+    </row>
+    <row r="70" spans="1:6">
+      <c r="A70" s="1">
+        <v>69</v>
+      </c>
+      <c r="B70" t="s">
+        <v>125</v>
+      </c>
+      <c r="C70">
+        <v>0</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="E70" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F70" s="6">
+        <v>200903</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6">
+      <c r="A71" s="1">
+        <v>70</v>
+      </c>
+      <c r="B71" t="s">
+        <v>126</v>
+      </c>
+      <c r="C71" s="4"/>
+      <c r="D71" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="E71" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F71" s="6">
+        <v>241028</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6">
+      <c r="A72" s="1">
+        <v>71</v>
+      </c>
+      <c r="B72" t="s">
+        <v>127</v>
+      </c>
+      <c r="C72">
+        <v>0</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="E72" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F72" s="6">
+        <v>241009</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6">
+      <c r="A73" s="1">
+        <v>72</v>
+      </c>
+      <c r="B73" t="s">
+        <v>128</v>
+      </c>
+      <c r="C73">
+        <v>0</v>
+      </c>
+      <c r="D73" s="2"/>
+      <c r="E73" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F73" s="6">
+        <v>241010</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6">
+      <c r="A74" s="1">
+        <v>73</v>
+      </c>
+      <c r="B74" t="s">
+        <v>129</v>
+      </c>
+      <c r="C74">
+        <v>0</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="E74" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F74" s="6">
+        <v>241023</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6">
+      <c r="A75" s="1">
+        <v>74</v>
+      </c>
+      <c r="B75" t="s">
+        <v>131</v>
+      </c>
+      <c r="C75">
+        <v>0</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="E75" s="5"/>
+      <c r="F75" s="6"/>
+    </row>
+    <row r="76" spans="1:6">
+      <c r="A76" s="1">
+        <v>75</v>
+      </c>
+      <c r="B76" t="s">
+        <v>132</v>
+      </c>
+      <c r="C76" s="4"/>
+      <c r="D76" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E76" s="5"/>
+      <c r="F76" s="6"/>
+    </row>
+    <row r="77" spans="1:6">
+      <c r="A77" s="1">
+        <v>76</v>
+      </c>
+      <c r="B77" t="s">
+        <v>133</v>
+      </c>
+      <c r="C77">
+        <v>0</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E77" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F77" s="6">
+        <v>240922</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6">
+      <c r="A78" s="1">
+        <v>77</v>
+      </c>
+      <c r="B78" t="s">
+        <v>135</v>
+      </c>
+      <c r="C78">
+        <v>0</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E78" s="5"/>
+      <c r="F78" s="6"/>
+    </row>
+    <row r="79" spans="1:6">
+      <c r="A79" s="1">
+        <v>78</v>
+      </c>
+      <c r="B79" t="s">
+        <v>136</v>
+      </c>
+      <c r="C79">
+        <v>0</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E79" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F79" s="6">
+        <v>200922</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6">
+      <c r="A80" s="1">
+        <v>79</v>
+      </c>
+      <c r="B80" t="s">
+        <v>137</v>
+      </c>
+      <c r="C80">
+        <v>0</v>
+      </c>
+      <c r="D80" s="2"/>
+      <c r="E80" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F80" s="6">
+        <v>241110</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6">
+      <c r="A81" s="1">
+        <v>80</v>
+      </c>
+      <c r="B81" t="s">
+        <v>138</v>
+      </c>
+      <c r="C81" s="4"/>
+      <c r="D81" s="2"/>
+      <c r="E81" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F81" s="6">
+        <v>241110</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6">
+      <c r="A82" s="1">
+        <v>81</v>
+      </c>
+      <c r="B82" t="s">
+        <v>140</v>
+      </c>
+      <c r="C82">
+        <v>0</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E82" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F82" s="6">
+        <v>240711</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6">
+      <c r="A83" s="1">
+        <v>82</v>
+      </c>
+      <c r="B83" t="s">
+        <v>142</v>
+      </c>
+      <c r="C83">
+        <v>0</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="E83" s="5"/>
+      <c r="F83" s="6"/>
+    </row>
+    <row r="84" spans="1:6">
+      <c r="A84" s="1">
+        <v>83</v>
+      </c>
+      <c r="B84" t="s">
+        <v>144</v>
+      </c>
+      <c r="C84">
+        <v>0</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="E84" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F84" s="6">
+        <v>241028</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6">
+      <c r="A85" s="1">
+        <v>84</v>
+      </c>
+      <c r="B85" t="s">
+        <v>146</v>
+      </c>
+      <c r="C85">
+        <v>0</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E85" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F85" s="6">
+        <v>201209</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6">
+      <c r="A86" s="1">
+        <v>85</v>
+      </c>
+      <c r="B86" t="s">
+        <v>147</v>
+      </c>
+      <c r="C86" s="4"/>
+      <c r="D86" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E86" s="5"/>
+      <c r="F86" s="6"/>
+    </row>
+    <row r="87" spans="1:6">
+      <c r="A87" s="1">
+        <v>86</v>
+      </c>
+      <c r="B87" t="s">
+        <v>149</v>
+      </c>
+      <c r="C87">
+        <v>0</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="E87" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F87" s="6">
+        <v>240923</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6">
+      <c r="A88" s="1">
+        <v>87</v>
+      </c>
+      <c r="B88" t="s">
+        <v>151</v>
+      </c>
+      <c r="C88">
+        <v>0</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="E88" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F88" s="6">
+        <v>230930</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6">
+      <c r="A89" s="1">
+        <v>88</v>
+      </c>
+      <c r="B89" t="s">
+        <v>153</v>
+      </c>
+      <c r="C89">
+        <v>0</v>
+      </c>
+      <c r="D89" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E89" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F89" s="6">
+        <v>241108</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6">
+      <c r="A90" s="1">
+        <v>89</v>
+      </c>
+      <c r="B90" t="s">
+        <v>155</v>
+      </c>
+      <c r="C90">
+        <v>0</v>
+      </c>
+      <c r="D90" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E90" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F90" s="6">
+        <v>241021</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6">
+      <c r="A91" s="1">
+        <v>90</v>
+      </c>
+      <c r="B91" t="s">
+        <v>157</v>
+      </c>
+      <c r="C91" s="4"/>
+      <c r="D91" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="E91" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F91" s="6">
+        <v>201119</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6">
+      <c r="A92" s="1">
+        <v>91</v>
+      </c>
+      <c r="B92" t="s">
+        <v>158</v>
+      </c>
+      <c r="C92">
+        <v>0</v>
+      </c>
+      <c r="D92" s="2"/>
+      <c r="E92" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F92" s="6">
+        <v>240828</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6">
+      <c r="A93" s="1">
+        <v>92</v>
+      </c>
+      <c r="B93" t="s">
+        <v>160</v>
+      </c>
+      <c r="C93">
+        <v>0</v>
+      </c>
+      <c r="D93" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E93" s="5"/>
+      <c r="F93" s="6"/>
+    </row>
+    <row r="94" spans="1:6">
+      <c r="A94" s="1">
+        <v>93</v>
+      </c>
+      <c r="B94" t="s">
+        <v>161</v>
+      </c>
+      <c r="C94">
+        <v>0</v>
+      </c>
+      <c r="D94" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E94" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F94" s="6">
+        <v>220809</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6">
+      <c r="C95" s="4"/>
+      <c r="D95" s="4"/>
+      <c r="E95" s="4"/>
+      <c r="F95" s="4"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B51" r:id="rId1" display="https://www.lyngsat.com/NSS-9.html"/>
+    <hyperlink ref="B52" r:id="rId2" display="https://www.lyngsat.com/Intelsat-18.html"/>
+    <hyperlink ref="B53" r:id="rId3" display="https://www.lyngsat.com/Eutelsat-172B.html"/>
+    <hyperlink ref="B54" r:id="rId4" display="https://www.lyngsat.com/Horizons-3e.html"/>
+    <hyperlink ref="B55" r:id="rId5" display="https://www.lyngsat.com/Intelsat-19.html"/>
+    <hyperlink ref="B56" r:id="rId6" display="https://www.lyngsat.com/ChinaSat-19.html"/>
+    <hyperlink ref="B57" r:id="rId7" display="https://www.lyngsat.com/Superbird-B3.html"/>
+    <hyperlink ref="B59" r:id="rId8" display="https://www.lyngsat.com/Measat-3a.html"/>
+    <hyperlink ref="B60" r:id="rId9" display="https://www.lyngsat.com/ABS-6.html"/>
+    <hyperlink ref="B62" r:id="rId10" display="https://www.lyngsat.com/Optus-10.html"/>
+    <hyperlink ref="B63" r:id="rId11" display="https://www.lyngsat.com/JCSAT-2B.html"/>
+    <hyperlink ref="B65" r:id="rId12" display="https://www.lyngsat.com/BRIsat.html"/>
+    <hyperlink ref="B66" r:id="rId13" display="https://www.lyngsat.com/JCSAT-1C.html"/>
+    <hyperlink ref="B67" r:id="rId14" display="https://www.lyngsat.com/Nusantara-Satu.html"/>
+    <hyperlink ref="B68" r:id="rId15" display="https://www.lyngsat.com/Express-AMU7.html"/>
+    <hyperlink ref="B69" r:id="rId16" display="https://www.lyngsat.com/JCSAT-16.html"/>
+    <hyperlink ref="B71" r:id="rId17" display="https://www.lyngsat.com/Apstar-9.html"/>
+    <hyperlink ref="B72" r:id="rId18" display="https://www.lyngsat.com/Express-AM5.html"/>
+    <hyperlink ref="B73" r:id="rId19" display="https://www.lyngsat.com/Express-AT2.html"/>
+    <hyperlink ref="B74" r:id="rId20" display="https://www.lyngsat.com/Telstar-18-Vantage.html"/>
+    <hyperlink ref="B75" r:id="rId21" display="https://www.lyngsat.com/Apstar-6E.html"/>
+    <hyperlink ref="B76" r:id="rId22" display="https://www.lyngsat.com/Apstar-6D.html"/>
+    <hyperlink ref="B77" r:id="rId23" display="https://www.lyngsat.com/Apstar-6C.html"/>
+    <hyperlink ref="B78" r:id="rId24" display="https://www.lyngsat.com/JCSAT-12.html"/>
+    <hyperlink ref="B79" r:id="rId25" display="https://www.lyngsat.com/JCSAT-5A.html"/>
+    <hyperlink ref="B80" r:id="rId26" display="https://www.lyngsat.com/Vinasat-1.html"/>
+    <hyperlink ref="B81" r:id="rId27" display="https://www.lyngsat.com/Vinasat-2.html"/>
+    <hyperlink ref="B82" r:id="rId28" display="https://www.lyngsat.com/ChinaSat-6C.html"/>
+    <hyperlink ref="B83" r:id="rId29" display="https://www.lyngsat.com/ChinaSat-2D.html"/>
+    <hyperlink ref="B84" r:id="rId30" display="https://www.lyngsat.com/LaoSat-1.html"/>
+    <hyperlink ref="B85" r:id="rId31" display="https://www.lyngsat.com/JCSAT-3A.html"/>
+    <hyperlink ref="B86" r:id="rId32" display="https://www.lyngsat.com/Cosmos-2526.html"/>
+    <hyperlink ref="B87" r:id="rId33" display="https://www.lyngsat.com/ChinaSat-6D.html"/>
+    <hyperlink ref="B88" r:id="rId34" display="https://www.lyngsat.com/JCSAT-4B.html"/>
+    <hyperlink ref="B89" r:id="rId35" display="https://www.lyngsat.com/AsiaSat-9.html"/>
+    <hyperlink ref="B90" r:id="rId36" display="https://www.lyngsat.com/AsiaSat-6-Thaicom-7.html"/>
+    <hyperlink ref="B91" r:id="rId37" display="https://www.lyngsat.com/Thaicom-4.html"/>
+    <hyperlink ref="B92" r:id="rId38" display="https://www.lyngsat.com/Bangabandhu-1.html"/>
+    <hyperlink ref="B93" r:id="rId39" display="https://www.lyngsat.com/ChinaSat-4A.html"/>
+    <hyperlink ref="B94" r:id="rId40" display="https://www.lyngsat.com/Telkom-3S.html"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="180" verticalDpi="180" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="180" verticalDpi="180" r:id="rId41"/>
 </worksheet>
 </file>
 

</xml_diff>